<commit_message>
Subindo Atualização das Tabelas e correção do código
</commit_message>
<xml_diff>
--- a/Backend/database/Censo 2022 - Escolaridade - SJC e SP.xlsx
+++ b/Backend/database/Censo 2022 - Escolaridade - SJC e SP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Downloads\Fatec\API\1 Semestre\tabelas\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF461887-FA0A-45E1-8896-F9EB6C855978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6393F217-A9E0-4CCF-8281-4C279007324F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1800" windowWidth="21600" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sem instrução e fundamental incompleto</t>
   </si>
@@ -39,25 +39,13 @@
     <t>Superior completo</t>
   </si>
   <si>
-    <t>Município</t>
-  </si>
-  <si>
-    <t>Sigla UF</t>
-  </si>
-  <si>
-    <t>Código do Município</t>
-  </si>
-  <si>
     <t xml:space="preserve">São José dos Campos </t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>Unidade da Federação</t>
-  </si>
-  <si>
-    <t>São Paulo</t>
+    <t>São Paulo (Estado)</t>
+  </si>
+  <si>
+    <t>Escolaridade</t>
   </si>
 </sst>
 </file>
@@ -93,9 +81,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,13 +438,12 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="36.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
@@ -453,89 +452,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>96985</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1">
+        <v>8420318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>74037</v>
       </c>
-      <c r="C2">
-        <v>228774</v>
-      </c>
-      <c r="D2">
-        <v>142053</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>3549904</v>
-      </c>
+      <c r="C3" s="1">
+        <v>5131662</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B4">
+        <v>228774</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13692410</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>8420318</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5131662</v>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>142053</v>
       </c>
       <c r="C5" s="1">
-        <v>13692410</v>
-      </c>
-      <c r="D5" s="1">
         <v>7478587</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>